<commit_message>
updated component diagram, added class diagramm
</commit_message>
<xml_diff>
--- a/docs/src/OC4-SGBD_Diagramme-de-classe.xlsx
+++ b/docs/src/OC4-SGBD_Diagramme-de-classe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="13860"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="13860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Draft" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>Client</t>
   </si>
@@ -303,6 +303,130 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>417604</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638175" y="371475"/>
+          <a:ext cx="11971429" cy="3695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>17584</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>46617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="4171950"/>
+          <a:ext cx="11733334" cy="8066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>636858</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>179858</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="190500"/>
+          <a:ext cx="10542858" cy="8942858"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,11 +1023,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -911,24 +1038,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>